<commit_message>
All done ready to make exe file
</commit_message>
<xml_diff>
--- a/output/records.xlsx
+++ b/output/records.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9168" yWindow="4380" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Records" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -516,27 +515,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>M-0001/24-25/LT</t>
+          <t>M-0001/25-26/LT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ADITYA NISHAD</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>RA PODAR COLLEGE OF COMMERCE AND ECONOMICS</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>BSC DATA SCIENCE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -544,524 +543,751 @@
           <t>75000</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>75000</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>56250</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>56250</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>18750</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>56250</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>56250</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>N S T P H C L</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>NTT</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ADITYA NISHAD</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>1234456</t>
+          <t>ADITYA NISHAD</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>14566</t>
+          <t>BANK OF BARODA</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>4522</t>
+          <t>456123</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>789456</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>456123</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>RAJ MORE</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M-0002/24-25/LT</t>
+          <t>M-0002/25-26/LT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ADITYA NISHAD</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>RA PODAR COLLEGE OF COMMERCE AND ECONOMICS</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>BSC DATA SCIENCE AND ANALYTICS</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>25000</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>25000</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>75000</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>56250</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>18750</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>6250</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>18750</t>
-        </is>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Eighteen Thousand, Seven Hundred And Fifty Only</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>I t t L t dU n i t e d w a y o f</t>
+          <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>NTT</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>ADITYA NISHAD</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>ADITYA NISHAD</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>13566</t>
+          <t>BANK OF BARODA</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>4545</t>
+          <t>456123</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2556</t>
+          <t>789456</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>741852</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>RAJ MORE</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>M-0003/24-25/LT</t>
+          <t>M-0003/25-26/LT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t xml:space="preserve">ADITYA NISHAD
+</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12th</t>
+          <t xml:space="preserve">RA PODAR COLLEGE OF COMMERCE AND ECONOMICS
+</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Aditya Nushad</t>
+          <t xml:space="preserve">BSC DATA SCIENCE
+</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>10000</t>
+          <t xml:space="preserve">75000
+</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Seven Thousand, Five Hundred Only</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>N S T P A s h o k C h h a b r a</t>
+          <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t>NTT</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t xml:space="preserve">ADITYA NISHAD
+</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>BOB123456</t>
+          <t xml:space="preserve">ADITYA NISHAD
+</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>112545</t>
+          <t>BOB</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>4864465</t>
+          <t>789456</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>6565464</t>
+          <t>456123</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>RAJMORE</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>M-0004/24-25/LT</t>
+          <t>M-0004/25-26/LT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t xml:space="preserve">ADITYA NISHAD
+</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12th</t>
+          <t xml:space="preserve">RA PODAR COLLEGE OF COMMERCE AND ECONOMICS
+</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Aditya Nushad</t>
+          <t xml:space="preserve">BSC DATA SCIENCE
+</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>10000</t>
+          <t xml:space="preserve">75000
+</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Seven Thousand, Five Hundred Only</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>N S T P A s h o k C h h a b r a</t>
+          <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t>NTT</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t xml:space="preserve">ADITYA NISHAD
+</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>BOB123456</t>
+          <t xml:space="preserve">ADITYA NISHAD
+</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>112545</t>
+          <t>BOB</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>4864465</t>
+          <t>789456</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>6565464</t>
+          <t>456123</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>RAJMORE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>M-0005/24-25/LT</t>
+          <t>M-0005/25-26/LT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t>ADITYA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>12th</t>
+          <t xml:space="preserve">PODAR </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Aditya Nushad</t>
+          <t>BSC</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>10000</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Seven Thousand, Five Hundred Only</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>N S T P A s h o k C h h a b r a</t>
+          <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t>NTT</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Aditya Nishad</t>
+          <t>ADITYA</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>BOB123456</t>
+          <t>ADITYA</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>112545</t>
+          <t>BOB</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>4864465</t>
+          <t>456123</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>6565464</t>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>741852</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>M-0006/24-25/LT</t>
+          <t>M-0006/25-26/LT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ascsfbw</t>
+          <t>ADITYA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ghfyuf</t>
+          <t xml:space="preserve">PODAR </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>iug8</t>
+          <t>BSC</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5000</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>5000</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3750</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>3750</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Three Thousand, Seven Hundred And Fifty Only</t>
+          <t>56250</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>N S T P</t>
+          <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>bug</t>
+          <t>NTT</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>yg87</t>
+          <t>ADITYA</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>iugyug</t>
+          <t>ADITYA</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>484</t>
+          <t>BOB</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>988</t>
+          <t>456123</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>9596</t>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>741852</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>03/12/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>M-0007/25-26/LT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ADITYA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PODAR</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>BSC</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>75000</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>75000</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>56250</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>18750</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>56250</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Fifty-Six Thousand, Two Hundred And Fifty Only</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Masoom</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>ADITYA</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>ADITYA</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>BOB</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>456123</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>415263</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>748596</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>RAJMORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03/12/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>M-0008/25-26/LT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ADITYA NISHAD</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RA PODAR </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BSC DATA </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>750000</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>750000</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>562500</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>187500</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>562500</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Five Lakh, Sixty-Two Thousand, Five Hundred Only</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>NTT</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>415263</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>BOB</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>748596</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>415263</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>789456</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>RAJ</t>
         </is>
       </c>
     </row>

</xml_diff>